<commit_message>
refactor: delete other branch,only leave main branch
</commit_message>
<xml_diff>
--- a/equipment_cyg/product/ceribell/ceribell_manual.xlsx
+++ b/equipment_cyg/product/ceribell/ceribell_manual.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="530" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="27915" windowHeight="12345" tabRatio="530" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="VID" sheetId="7" state="hidden" r:id="rId1"/>
     <sheet name="sv_ids" sheetId="9" r:id="rId2"/>
     <sheet name="plc" sheetId="13" r:id="rId3"/>
-    <sheet name="Recipe" sheetId="8" state="hidden" r:id="rId4"/>
-    <sheet name="RCMD" sheetId="6" state="hidden" r:id="rId5"/>
-    <sheet name="SECS定义协议" sheetId="10" state="hidden" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId4"/>
+    <sheet name="Recipe" sheetId="8" state="hidden" r:id="rId5"/>
+    <sheet name="RCMD" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="SECS定义协议" sheetId="10" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">plc!$E$1:$E$43</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="269">
   <si>
     <t>VID</t>
   </si>
@@ -482,6 +483,9 @@
   </si>
   <si>
     <t>出站mes检查结果信号</t>
+  </si>
+  <si>
+    <t>写入MES反馈结果</t>
   </si>
   <si>
     <t>功能</t>
@@ -913,7 +917,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1009,6 +1013,18 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1842,137 +1858,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2199,9 +2215,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2214,16 +2227,28 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2602,7 +2627,7 @@
   <cols>
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="29.375" customWidth="1"/>
-    <col min="3" max="3" width="5.375" style="85" customWidth="1"/>
+    <col min="3" max="3" width="5.375" style="88" customWidth="1"/>
     <col min="4" max="4" width="29.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2618,10 +2643,10 @@
       </c>
     </row>
     <row r="2" ht="16.5" spans="1:3">
-      <c r="A2" s="86">
+      <c r="A2" s="89">
         <v>0</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="90" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -2629,16 +2654,16 @@
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:4">
-      <c r="A3" s="86">
+      <c r="A3" s="89">
         <v>1</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="89" t="s">
+      <c r="D3" s="92" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2646,13 +2671,13 @@
       <c r="A4" s="75">
         <v>10</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="90" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="89"/>
+      <c r="D4" s="92"/>
     </row>
     <row r="5" ht="16.5" spans="1:4">
       <c r="A5" s="75">
@@ -2664,7 +2689,7 @@
       <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="89"/>
+      <c r="D5" s="92"/>
     </row>
     <row r="6" ht="16.5" spans="1:4">
       <c r="A6" s="75">
@@ -2676,7 +2701,7 @@
       <c r="C6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="89"/>
+      <c r="D6" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2700,332 +2725,332 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="81" customWidth="1"/>
-    <col min="2" max="2" width="34.625" style="81" customWidth="1"/>
-    <col min="3" max="3" width="21.375" style="81" customWidth="1"/>
-    <col min="4" max="4" width="24.625" style="81" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="81"/>
+    <col min="1" max="1" width="9.125" style="84" customWidth="1"/>
+    <col min="2" max="2" width="34.625" style="84" customWidth="1"/>
+    <col min="3" max="3" width="21.375" style="84" customWidth="1"/>
+    <col min="4" max="4" width="24.625" style="84" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="84"/>
   </cols>
   <sheetData>
-    <row r="1" s="81" customFormat="1" spans="1:4">
-      <c r="A1" s="83" t="s">
+    <row r="1" s="84" customFormat="1" spans="1:4">
+      <c r="A1" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="86" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" s="82" customFormat="1" spans="1:4">
-      <c r="A2" s="84">
+    <row r="2" s="85" customFormat="1" spans="1:4">
+      <c r="A2" s="87">
         <v>500</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="87" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" s="82" customFormat="1" spans="1:4">
-      <c r="A3" s="84">
+    <row r="3" s="85" customFormat="1" spans="1:4">
+      <c r="A3" s="87">
         <v>503</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="87" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" s="82" customFormat="1" spans="1:4">
-      <c r="A4" s="84">
+    <row r="4" s="85" customFormat="1" spans="1:4">
+      <c r="A4" s="87">
         <v>504</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="84" t="s">
+      <c r="D4" s="87" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" s="82" customFormat="1" spans="1:4">
-      <c r="A5" s="84">
+    <row r="5" s="85" customFormat="1" spans="1:4">
+      <c r="A5" s="87">
         <v>505</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="87" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" s="82" customFormat="1" spans="1:4">
-      <c r="A6" s="84">
+    <row r="6" s="85" customFormat="1" spans="1:4">
+      <c r="A6" s="87">
         <v>506</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="87" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" s="82" customFormat="1" spans="1:4">
-      <c r="A7" s="84">
+    <row r="7" s="85" customFormat="1" spans="1:4">
+      <c r="A7" s="87">
         <v>507</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="87" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" s="82" customFormat="1" spans="1:4">
-      <c r="A8" s="84">
+    <row r="8" s="85" customFormat="1" spans="1:4">
+      <c r="A8" s="87">
         <v>508</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="87" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" s="82" customFormat="1" spans="1:4">
-      <c r="A9" s="84">
+    <row r="9" s="85" customFormat="1" spans="1:4">
+      <c r="A9" s="87">
         <v>509</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="84" t="s">
+      <c r="D9" s="87" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" s="82" customFormat="1" spans="1:4">
-      <c r="A10" s="84">
+    <row r="10" s="85" customFormat="1" spans="1:4">
+      <c r="A10" s="87">
         <v>510</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="87" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" s="82" customFormat="1" spans="1:4">
-      <c r="A11" s="84">
+    <row r="11" s="85" customFormat="1" spans="1:4">
+      <c r="A11" s="87">
         <v>511</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="87" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" s="82" customFormat="1" spans="1:4">
-      <c r="A12" s="84">
+    <row r="12" s="85" customFormat="1" spans="1:4">
+      <c r="A12" s="87">
         <v>512</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="87" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" s="82" customFormat="1" spans="1:4">
-      <c r="A13" s="84">
+    <row r="13" s="85" customFormat="1" spans="1:4">
+      <c r="A13" s="87">
         <v>513</v>
       </c>
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="87" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" s="82" customFormat="1" spans="1:4">
-      <c r="A14" s="84">
+    <row r="14" s="85" customFormat="1" spans="1:4">
+      <c r="A14" s="87">
         <v>514</v>
       </c>
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="84" t="s">
+      <c r="D14" s="87" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" s="82" customFormat="1" spans="1:4">
-      <c r="A15" s="84">
+    <row r="15" s="85" customFormat="1" spans="1:4">
+      <c r="A15" s="87">
         <v>515</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="84" t="s">
+      <c r="D15" s="87" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" s="82" customFormat="1" spans="1:4">
-      <c r="A16" s="84">
+    <row r="16" s="85" customFormat="1" spans="1:4">
+      <c r="A16" s="87">
         <v>516</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="84" t="s">
+      <c r="C16" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="84" t="s">
+      <c r="D16" s="87" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" s="82" customFormat="1" spans="1:4">
-      <c r="A17" s="84">
+    <row r="17" s="85" customFormat="1" spans="1:4">
+      <c r="A17" s="87">
         <v>517</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="84" t="s">
+      <c r="C17" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="84" t="s">
+      <c r="D17" s="87" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" s="82" customFormat="1" spans="1:4">
-      <c r="A18" s="84">
+    <row r="18" s="85" customFormat="1" spans="1:4">
+      <c r="A18" s="87">
         <v>518</v>
       </c>
-      <c r="B18" s="84" t="s">
+      <c r="B18" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="84" t="s">
+      <c r="C18" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="84" t="s">
+      <c r="D18" s="87" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" s="82" customFormat="1" spans="1:4">
-      <c r="A19" s="84">
+    <row r="19" s="85" customFormat="1" spans="1:4">
+      <c r="A19" s="87">
         <v>519</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="84" t="s">
+      <c r="C19" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="84" t="s">
+      <c r="D19" s="87" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" s="82" customFormat="1" spans="1:4">
-      <c r="A20" s="84">
+    <row r="20" s="85" customFormat="1" spans="1:4">
+      <c r="A20" s="87">
         <v>520</v>
       </c>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="84" t="s">
+      <c r="C20" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="84" t="s">
+      <c r="D20" s="87" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" s="82" customFormat="1" spans="1:4">
-      <c r="A21" s="84">
+    <row r="21" s="85" customFormat="1" spans="1:4">
+      <c r="A21" s="87">
         <v>521</v>
       </c>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="84" t="s">
+      <c r="C21" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="84" t="s">
+      <c r="D21" s="87" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" s="82" customFormat="1" spans="1:4">
-      <c r="A22" s="84">
+    <row r="22" s="85" customFormat="1" spans="1:4">
+      <c r="A22" s="87">
         <v>522</v>
       </c>
-      <c r="B22" s="84" t="s">
+      <c r="B22" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="84" t="s">
+      <c r="C22" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="84" t="s">
+      <c r="D22" s="87" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" s="82" customFormat="1" spans="1:4">
-      <c r="A23" s="84">
+    <row r="23" s="85" customFormat="1" spans="1:4">
+      <c r="A23" s="87">
         <v>523</v>
       </c>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="84" t="s">
+      <c r="D23" s="87" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3041,10 +3066,10 @@
   <sheetPr/>
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="A1:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -3057,669 +3082,669 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="76" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A2" s="78" t="s">
+    <row r="2" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A2" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="80"/>
-    </row>
-    <row r="3" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A3" s="79" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
+    </row>
+    <row r="3" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A3" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A4" s="78" t="s">
+    <row r="4" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A4" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="80"/>
-    </row>
-    <row r="5" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A5" s="79" t="s">
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
+    </row>
+    <row r="5" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A5" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A6" s="79" t="s">
+    <row r="6" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A6" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="78" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A7" s="79" t="s">
+    <row r="7" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A7" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="79" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A8" s="79" t="s">
+    <row r="8" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A8" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A9" s="78" t="s">
+    <row r="9" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A9" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="80"/>
-    </row>
-    <row r="10" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A10" s="79" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="79"/>
+    </row>
+    <row r="10" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A10" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="79" t="s">
+      <c r="D10" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="80" t="s">
+      <c r="E10" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A11" s="79" t="s">
+    <row r="11" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A11" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="79" t="s">
+      <c r="D11" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="80" t="s">
+      <c r="E11" s="79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A12" s="79" t="s">
+    <row r="12" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A12" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="79" t="s">
+      <c r="D12" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="80" t="s">
+      <c r="E12" s="79" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A13" s="79" t="s">
+    <row r="13" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A13" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="80" t="s">
+      <c r="E13" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A14" s="78" t="s">
+    <row r="14" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A14" s="77" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="80"/>
-    </row>
-    <row r="15" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A15" s="79" t="s">
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="79"/>
+    </row>
+    <row r="15" s="83" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A15" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="79" t="s">
+      <c r="C15" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="79" t="s">
+      <c r="D15" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="80" t="s">
+      <c r="E15" s="81" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A16" s="79" t="s">
+    <row r="16" s="83" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A16" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="79" t="s">
+      <c r="B16" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="79" t="s">
+      <c r="C16" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="79" t="s">
+      <c r="D16" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="80" t="s">
+      <c r="E16" s="81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A17" s="79" t="s">
+    <row r="17" s="83" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A17" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="79" t="s">
+      <c r="D17" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="80" t="s">
+      <c r="E17" s="81" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A18" s="78" t="s">
+    <row r="18" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A18" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
-    </row>
-    <row r="19" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A19" s="79" t="s">
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="79"/>
+    </row>
+    <row r="19" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A19" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="79" t="s">
+      <c r="D19" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="80" t="s">
+      <c r="E19" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A20" s="79" t="s">
+    <row r="20" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A20" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="79" t="s">
+      <c r="D20" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="80" t="s">
+      <c r="E20" s="79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A21" s="79" t="s">
+    <row r="21" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A21" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="79" t="s">
+      <c r="C21" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="79" t="s">
+      <c r="D21" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="80" t="s">
+      <c r="E21" s="79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A22" s="79" t="s">
+    <row r="22" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A22" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="79" t="s">
+      <c r="B22" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="79" t="s">
+      <c r="D22" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="80" t="s">
+      <c r="E22" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A23" s="79" t="s">
+    <row r="23" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A23" s="78" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="79" t="s">
+      <c r="D23" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="80" t="s">
+      <c r="E23" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="24" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A24" s="79" t="s">
+    <row r="24" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A24" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="79" t="s">
+      <c r="C24" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="79" t="s">
+      <c r="D24" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="80" t="s">
+      <c r="E24" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A25" s="79" t="s">
+    <row r="25" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A25" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="79" t="s">
+      <c r="B25" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="C25" s="79" t="s">
+      <c r="C25" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="79" t="s">
+      <c r="D25" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="80" t="s">
+      <c r="E25" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A26" s="78" t="s">
+    <row r="26" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A26" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="80"/>
-    </row>
-    <row r="27" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A27" s="79" t="s">
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="79"/>
+    </row>
+    <row r="27" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A27" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="79" t="s">
+      <c r="C27" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="79" t="s">
+      <c r="D27" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="80" t="s">
+      <c r="E27" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A28" s="79" t="s">
+    <row r="28" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A28" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="79" t="s">
+      <c r="B28" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="79" t="s">
+      <c r="C28" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="79" t="s">
+      <c r="D28" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="80" t="s">
+      <c r="E28" s="79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="29" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A29" s="79" t="s">
+    <row r="29" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A29" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="79" t="s">
+      <c r="C29" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="79" t="s">
+      <c r="D29" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="80" t="s">
+      <c r="E29" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A30" s="79" t="s">
+    <row r="30" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A30" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="79" t="s">
+      <c r="C30" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="79" t="s">
+      <c r="D30" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="80" t="s">
+      <c r="E30" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="31" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A31" s="79" t="s">
+    <row r="31" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A31" s="78" t="s">
         <v>126</v>
       </c>
-      <c r="B31" s="79" t="s">
+      <c r="B31" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="C31" s="79" t="s">
+      <c r="C31" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="79" t="s">
+      <c r="D31" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="80" t="s">
+      <c r="E31" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A32" s="79" t="s">
+    <row r="32" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A32" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="B32" s="79" t="s">
+      <c r="B32" s="78" t="s">
         <v>129</v>
       </c>
-      <c r="C32" s="79" t="s">
+      <c r="C32" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="79" t="s">
+      <c r="D32" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="80" t="s">
+      <c r="E32" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="33" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A33" s="79" t="s">
+    <row r="33" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A33" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="78" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="79" t="s">
+      <c r="C33" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="79" t="s">
+      <c r="D33" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="80" t="s">
+      <c r="E33" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A34" s="78" t="s">
+    <row r="34" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A34" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="79"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="80"/>
-    </row>
-    <row r="35" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A35" s="79" t="s">
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="79"/>
+    </row>
+    <row r="35" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A35" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="C35" s="79" t="s">
+      <c r="C35" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="79" t="s">
+      <c r="D35" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="80" t="s">
+      <c r="E35" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A36" s="79" t="s">
+    <row r="36" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A36" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="B36" s="79" t="s">
+      <c r="B36" s="78" t="s">
         <v>135</v>
       </c>
-      <c r="C36" s="79" t="s">
+      <c r="C36" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="79" t="s">
+      <c r="D36" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="80" t="s">
+      <c r="E36" s="79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A37" s="79" t="s">
+    <row r="37" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A37" s="78" t="s">
         <v>136</v>
       </c>
-      <c r="B37" s="79" t="s">
+      <c r="B37" s="78" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="79" t="s">
+      <c r="C37" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="79" t="s">
+      <c r="D37" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="80" t="s">
+      <c r="E37" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="38" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A38" s="78" t="s">
+    <row r="38" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A38" s="77" t="s">
         <v>138</v>
       </c>
-      <c r="B38" s="79"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="80"/>
-    </row>
-    <row r="39" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A39" s="79" t="s">
+      <c r="B38" s="78"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="79"/>
+    </row>
+    <row r="39" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A39" s="78" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="C39" s="79" t="s">
+      <c r="C39" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="79" t="s">
+      <c r="D39" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E39" s="80" t="s">
+      <c r="E39" s="79" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A40" s="79" t="s">
+    <row r="40" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A40" s="78" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="79" t="s">
+      <c r="B40" s="78" t="s">
         <v>142</v>
       </c>
-      <c r="C40" s="79" t="s">
+      <c r="C40" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="79" t="s">
+      <c r="D40" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="80" t="s">
+      <c r="E40" s="79" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A41" s="79" t="s">
+    <row r="41" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A41" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="B41" s="79" t="s">
+      <c r="B41" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="79" t="s">
+      <c r="C41" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="79" t="s">
+      <c r="D41" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="80" t="s">
+      <c r="E41" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A42" s="79" t="s">
+    <row r="42" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A42" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="B42" s="79" t="s">
+      <c r="B42" s="78" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="79" t="s">
+      <c r="C42" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="79" t="s">
+      <c r="D42" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E42" s="80" t="s">
+      <c r="E42" s="79" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" s="76" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A43" s="79" t="s">
+    <row r="43" s="82" customFormat="1" ht="18.75" spans="1:5">
+      <c r="A43" s="78" t="s">
         <v>147</v>
       </c>
-      <c r="B43" s="79" t="s">
+      <c r="B43" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C43" s="79" t="s">
+      <c r="C43" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="79" t="s">
+      <c r="D43" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="80" t="s">
+      <c r="E43" s="79" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3731,6 +3756,713 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="50.375" customWidth="1"/>
+    <col min="2" max="2" width="49.625" customWidth="1"/>
+    <col min="3" max="3" width="5.125" customWidth="1"/>
+    <col min="5" max="5" width="8.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" ht="18.75" spans="1:5">
+      <c r="A2" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
+    </row>
+    <row r="3" ht="18.75" spans="1:5">
+      <c r="A3" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" ht="18.75" spans="1:5">
+      <c r="A4" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
+    </row>
+    <row r="5" ht="18.75" spans="1:5">
+      <c r="A5" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" ht="18.75" spans="1:5">
+      <c r="A6" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="78" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" ht="18.75" spans="1:5">
+      <c r="A7" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="79" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" ht="18.75" spans="1:5">
+      <c r="A8" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" ht="18.75" spans="1:5">
+      <c r="A9" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="79"/>
+    </row>
+    <row r="10" ht="18.75" spans="1:5">
+      <c r="A10" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" ht="18.75" spans="1:5">
+      <c r="A11" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" ht="18.75" spans="1:5">
+      <c r="A12" s="78" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="78" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="79" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" ht="18.75" spans="1:5">
+      <c r="A13" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" ht="18.75" spans="1:5">
+      <c r="A14" s="77" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="79"/>
+    </row>
+    <row r="15" ht="18.75" spans="1:5">
+      <c r="A15" s="80" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="80" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" ht="18.75" spans="1:5">
+      <c r="A16" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="80" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" ht="18.75" spans="1:5">
+      <c r="A17" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="80" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="81" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" ht="18.75" spans="1:5">
+      <c r="A18" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="80" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75" spans="1:5">
+      <c r="A19" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="79"/>
+    </row>
+    <row r="20" ht="18.75" spans="1:5">
+      <c r="A20" s="78" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="78" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" ht="18.75" spans="1:5">
+      <c r="A21" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" ht="18.75" spans="1:5">
+      <c r="A22" s="78" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="78" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" ht="18.75" spans="1:5">
+      <c r="A23" s="78" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="78" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" ht="18.75" spans="1:5">
+      <c r="A24" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" ht="18.75" spans="1:5">
+      <c r="A25" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" ht="18.75" spans="1:5">
+      <c r="A26" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="78" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" ht="18.75" spans="1:5">
+      <c r="A27" s="77" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="79"/>
+    </row>
+    <row r="28" ht="18.75" spans="1:5">
+      <c r="A28" s="78" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" ht="18.75" spans="1:5">
+      <c r="A29" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" ht="18.75" spans="1:5">
+      <c r="A30" s="78" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" ht="18.75" spans="1:5">
+      <c r="A31" s="78" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="78" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" ht="18.75" spans="1:5">
+      <c r="A32" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="78" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" ht="18.75" spans="1:5">
+      <c r="A33" s="78" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="78" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" ht="18.75" spans="1:5">
+      <c r="A34" s="78" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="78" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" ht="18.75" spans="1:5">
+      <c r="A35" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="78"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="79"/>
+    </row>
+    <row r="36" ht="18.75" spans="1:5">
+      <c r="A36" s="78" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" ht="18.75" spans="1:5">
+      <c r="A37" s="78" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="78" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" ht="18.75" spans="1:5">
+      <c r="A38" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" ht="18.75" spans="1:5">
+      <c r="A39" s="77" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="78"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="79"/>
+    </row>
+    <row r="40" ht="18.75" spans="1:5">
+      <c r="A40" s="78" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" ht="18.75" spans="1:5">
+      <c r="A41" s="78" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="78" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" s="79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" ht="18.75" spans="1:5">
+      <c r="A42" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" ht="18.75" spans="1:5">
+      <c r="A43" s="78" t="s">
+        <v>145</v>
+      </c>
+      <c r="B43" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="79" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" ht="18.75" spans="1:5">
+      <c r="A44" s="78" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="78" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F9"/>
@@ -3750,41 +4482,41 @@
   <sheetData>
     <row r="1" ht="21" spans="1:5">
       <c r="A1" s="74" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B1" s="74" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C1" s="74" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E1" s="74" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" ht="21" spans="1:5">
       <c r="A2" s="74" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E2" s="75" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" ht="21" spans="1:5">
       <c r="A3" s="74" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B3" s="14">
         <v>5</v>
@@ -3801,44 +4533,44 @@
     </row>
     <row r="4" ht="21" spans="1:6">
       <c r="A4" s="74" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E4" s="75" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" ht="21" spans="1:5">
       <c r="A5" s="74" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E5" s="75" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" ht="21" spans="1:5">
       <c r="A6" s="74" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
@@ -3855,22 +4587,22 @@
     </row>
     <row r="7" ht="21" spans="1:5">
       <c r="A7" s="74" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="75" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" ht="21" spans="1:5">
       <c r="A8" s="74" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B8" s="75">
         <v>0</v>
@@ -3887,7 +4619,7 @@
     </row>
     <row r="9" ht="21" spans="1:5">
       <c r="A9" s="74" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B9" s="75">
         <v>0</v>
@@ -3908,7 +4640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G21"/>
@@ -3930,13 +4662,13 @@
   <sheetData>
     <row r="1" ht="14.25" spans="1:7">
       <c r="A1" s="53" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D1" s="56"/>
       <c r="E1" s="57"/>
@@ -3949,16 +4681,16 @@
       <c r="A2" s="59"/>
       <c r="B2" s="60"/>
       <c r="C2" s="61" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E2" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="62" t="s">
         <v>174</v>
-      </c>
-      <c r="F2" s="62" t="s">
-        <v>173</v>
       </c>
       <c r="G2" s="63"/>
     </row>
@@ -3967,23 +4699,23 @@
         <v>4000</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D3" s="66"/>
       <c r="E3" s="67"/>
       <c r="F3" s="64"/>
       <c r="G3" s="67" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="64"/>
       <c r="B4" s="68"/>
       <c r="C4" s="66" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D4" s="66"/>
       <c r="E4" s="67"/>
@@ -3995,16 +4727,16 @@
         <v>4001</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" s="66"/>
       <c r="E5" s="67"/>
       <c r="F5" s="64"/>
       <c r="G5" s="67" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4012,23 +4744,23 @@
         <v>4002</v>
       </c>
       <c r="B6" s="70" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D6" s="66"/>
       <c r="E6" s="67"/>
       <c r="F6" s="64"/>
       <c r="G6" s="69" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="71"/>
       <c r="B7" s="68"/>
       <c r="C7" s="66" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D7" s="66"/>
       <c r="E7" s="67"/>
@@ -4039,10 +4771,10 @@
       <c r="A8" s="71"/>
       <c r="B8" s="68"/>
       <c r="C8" s="66" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E8" s="67"/>
       <c r="F8" s="64"/>
@@ -4052,7 +4784,7 @@
       <c r="A9" s="72"/>
       <c r="B9" s="73"/>
       <c r="C9" s="66" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D9" s="66"/>
       <c r="E9" s="66"/>
@@ -4064,13 +4796,13 @@
         <v>4003</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E10" s="66"/>
       <c r="F10" s="66"/>
@@ -4080,10 +4812,10 @@
       <c r="A11" s="72"/>
       <c r="B11" s="73"/>
       <c r="C11" s="66" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D11" s="66" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E11" s="66"/>
       <c r="F11" s="66"/>
@@ -4094,10 +4826,10 @@
         <v>4004</v>
       </c>
       <c r="B12" s="70" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D12" s="66"/>
       <c r="E12" s="66"/>
@@ -4108,7 +4840,7 @@
       <c r="A13" s="72"/>
       <c r="B13" s="73"/>
       <c r="C13" s="66" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D13" s="66"/>
       <c r="E13" s="66"/>
@@ -4120,10 +4852,10 @@
         <v>4005</v>
       </c>
       <c r="B14" s="70" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C14" s="66" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D14" s="66"/>
       <c r="E14" s="66"/>
@@ -4134,7 +4866,7 @@
       <c r="A15" s="72"/>
       <c r="B15" s="73"/>
       <c r="C15" s="66" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D15" s="66"/>
       <c r="E15" s="66"/>
@@ -4146,10 +4878,10 @@
         <v>4006</v>
       </c>
       <c r="B16" s="70" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C16" s="66" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D16" s="66"/>
       <c r="E16" s="66"/>
@@ -4160,7 +4892,7 @@
       <c r="A17" s="72"/>
       <c r="B17" s="73"/>
       <c r="C17" s="66" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D17" s="66"/>
       <c r="E17" s="66"/>
@@ -4172,10 +4904,10 @@
         <v>4007</v>
       </c>
       <c r="B18" s="70" t="s">
+        <v>200</v>
+      </c>
+      <c r="C18" s="66" t="s">
         <v>199</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>198</v>
       </c>
       <c r="D18" s="66"/>
       <c r="E18" s="66"/>
@@ -4186,7 +4918,7 @@
       <c r="A19" s="72"/>
       <c r="B19" s="73"/>
       <c r="C19" s="66" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D19" s="66"/>
       <c r="E19" s="66"/>
@@ -4198,10 +4930,10 @@
         <v>4008</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C20" s="66" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D20" s="66"/>
       <c r="E20" s="67"/>
@@ -4212,7 +4944,7 @@
       <c r="A21" s="72"/>
       <c r="B21" s="73"/>
       <c r="C21" s="66" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D21" s="66"/>
       <c r="E21" s="67"/>
@@ -4250,7 +4982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="D1:N55"/>
@@ -4277,18 +5009,18 @@
   <sheetData>
     <row r="1" ht="21.75" spans="4:4">
       <c r="D1" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" ht="16.5" spans="4:9">
       <c r="D2" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>0</v>
@@ -4305,7 +5037,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
@@ -4314,7 +5046,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I3" s="40" t="s">
         <v>5</v>
@@ -4326,7 +5058,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I4" s="41"/>
     </row>
@@ -4336,7 +5068,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I5" s="41"/>
     </row>
@@ -4346,7 +5078,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I6" s="41"/>
     </row>
@@ -4356,7 +5088,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I7" s="42"/>
     </row>
@@ -4365,7 +5097,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
@@ -4374,13 +5106,13 @@
         <v>2</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I8" s="40" t="s">
         <v>3</v>
       </c>
       <c r="K8" s="43" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>1</v>
@@ -4393,7 +5125,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I9" s="41"/>
       <c r="K9" s="14">
@@ -4403,7 +5135,7 @@
         <v>5</v>
       </c>
       <c r="M9" s="45" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" ht="16.5" spans="4:13">
@@ -4412,13 +5144,13 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I10" s="41"/>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="45" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" ht="16.5" spans="4:13">
@@ -4427,13 +5159,13 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I11" s="42"/>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="45" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" ht="16.5" spans="4:13">
@@ -4441,7 +5173,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F12" s="12">
         <v>3</v>
@@ -4450,15 +5182,15 @@
         <v>3</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="45" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" ht="16.5" spans="4:13">
@@ -4466,7 +5198,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F13" s="15">
         <v>4</v>
@@ -4475,15 +5207,15 @@
         <v>4</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="46" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" ht="16.5" spans="4:13">
@@ -4494,10 +5226,10 @@
         <v>5</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K14" s="14">
         <v>2</v>
@@ -4506,7 +5238,7 @@
         <v>3</v>
       </c>
       <c r="M14" s="45" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" ht="16.5" spans="4:13">
@@ -4514,7 +5246,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F15" s="15">
         <v>5</v>
@@ -4523,15 +5255,15 @@
         <v>4</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="45" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" ht="16.5" spans="4:13">
@@ -4542,15 +5274,15 @@
         <v>5</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="45" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" ht="16.5" spans="4:13">
@@ -4561,15 +5293,15 @@
         <v>6</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
       <c r="M17" s="46" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" ht="16.5" spans="4:13">
@@ -4577,7 +5309,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F18" s="15">
         <v>6</v>
@@ -4586,19 +5318,19 @@
         <v>4</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K18" s="11">
         <v>3</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M18" s="46" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" ht="16.5" spans="4:13">
@@ -4606,7 +5338,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
@@ -4616,10 +5348,10 @@
         <v>4</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M19" s="46" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" ht="16.5" spans="4:9">
@@ -4627,7 +5359,7 @@
         <v>8</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F20" s="15">
         <v>8</v>
@@ -4636,10 +5368,10 @@
         <v>8</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" ht="16.5" spans="4:9">
@@ -4647,7 +5379,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -4659,7 +5391,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F22" s="16">
         <v>10</v>
@@ -4668,10 +5400,10 @@
         <v>10</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" ht="16.5" spans="4:9">
@@ -4698,16 +5430,16 @@
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
       <c r="K25" s="47" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L25" s="48" t="s">
         <v>1</v>
       </c>
       <c r="M25" s="48" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="N25" s="48" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" ht="32.25" spans="4:14">
@@ -4718,20 +5450,20 @@
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
       <c r="K26" s="49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L26" s="50" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M26" s="50"/>
       <c r="N26" s="50" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" ht="16.5" spans="4:14">
       <c r="D27" s="11"/>
       <c r="E27" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
@@ -4741,17 +5473,17 @@
         <v>0</v>
       </c>
       <c r="L27" s="50" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="M27" s="50"/>
       <c r="N27" s="50" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" ht="16.5" spans="4:9">
       <c r="D28" s="23"/>
       <c r="E28" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -4761,45 +5493,45 @@
     <row r="37" ht="14.25"/>
     <row r="38" ht="16.5" spans="4:10">
       <c r="D38" s="24" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F38" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="I38" s="51" t="s">
         <v>244</v>
       </c>
-      <c r="G38" s="25" t="s">
-        <v>245</v>
-      </c>
-      <c r="H38" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="I38" s="51" t="s">
-        <v>243</v>
-      </c>
       <c r="J38" s="52" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="39" ht="16.5" spans="4:10">
       <c r="D39" s="27" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H39" s="11">
         <v>1</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="J39" s="12">
         <v>2</v>
@@ -4809,14 +5541,14 @@
       <c r="D40" s="30"/>
       <c r="E40" s="31"/>
       <c r="F40" s="29" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="11">
         <v>2</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="J40" s="12">
         <v>2</v>
@@ -4826,7 +5558,7 @@
       <c r="D41" s="30"/>
       <c r="E41" s="31"/>
       <c r="F41" s="32" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G41" s="31"/>
     </row>
@@ -4834,7 +5566,7 @@
       <c r="D42" s="30"/>
       <c r="E42" s="31"/>
       <c r="F42" s="33" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G42" s="31"/>
     </row>
@@ -4842,7 +5574,7 @@
       <c r="D43" s="30"/>
       <c r="E43" s="31"/>
       <c r="F43" s="33" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G43" s="31"/>
     </row>
@@ -4850,7 +5582,7 @@
       <c r="D44" s="30"/>
       <c r="E44" s="31"/>
       <c r="F44" s="33" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G44" s="31"/>
     </row>
@@ -4858,7 +5590,7 @@
       <c r="D45" s="30"/>
       <c r="E45" s="31"/>
       <c r="F45" s="33" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G45" s="31"/>
     </row>
@@ -4866,7 +5598,7 @@
       <c r="D46" s="30"/>
       <c r="E46" s="31"/>
       <c r="F46" s="33" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G46" s="31"/>
     </row>
@@ -4874,7 +5606,7 @@
       <c r="D47" s="30"/>
       <c r="E47" s="31"/>
       <c r="F47" s="33" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G47" s="31"/>
     </row>
@@ -4882,7 +5614,7 @@
       <c r="D48" s="30"/>
       <c r="E48" s="31"/>
       <c r="F48" s="33" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G48" s="31"/>
     </row>
@@ -4890,7 +5622,7 @@
       <c r="D49" s="30"/>
       <c r="E49" s="31"/>
       <c r="F49" s="33" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G49" s="31"/>
     </row>
@@ -4898,7 +5630,7 @@
       <c r="D50" s="30"/>
       <c r="E50" s="31"/>
       <c r="F50" s="33" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G50" s="31"/>
     </row>
@@ -4906,7 +5638,7 @@
       <c r="D51" s="30"/>
       <c r="E51" s="31"/>
       <c r="F51" s="33" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G51" s="31"/>
     </row>
@@ -4914,23 +5646,23 @@
       <c r="D52" s="34"/>
       <c r="E52" s="35"/>
       <c r="F52" s="36" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G52" s="35"/>
     </row>
     <row r="53" ht="21" spans="4:4">
       <c r="D53" s="37" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" ht="15.75" spans="4:4">
       <c r="D54" s="38" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="55" ht="15.75" spans="4:4">
       <c r="D55" s="39" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>